<commit_message>
step 5 half done
</commit_message>
<xml_diff>
--- a/bot_outputs/step_5_out.xlsx
+++ b/bot_outputs/step_5_out.xlsx
@@ -22,8 +22,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,###"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -72,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -82,8 +84,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3520,6 +3525,70 @@
           <t>Oil Differential (%)</t>
         </is>
       </c>
+      <c r="E62" s="11">
+        <f>IFERROR(E54/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F62" s="11">
+        <f>IFERROR(F54/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G62" s="11">
+        <f>IFERROR(G54/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H62" s="11">
+        <f>IFERROR(H54/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I62" s="11">
+        <f>IFERROR(I54/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J62" s="11">
+        <f>IFERROR(J54/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K62" s="11">
+        <f>IFERROR(K54/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L62" s="11">
+        <f>IFERROR(L54/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M62" s="11">
+        <f>IFERROR(M54/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N62" s="11">
+        <f>IFERROR(N54/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O62" s="11">
+        <f>IFERROR(O54/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P62" s="11">
+        <f>IFERROR(P54/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q62" s="11">
+        <f>IFERROR(AVERAGE(N62:P62),"")</f>
+        <v/>
+      </c>
+      <c r="R62" s="11">
+        <f>IFERROR(AVERAGE(K62:P62),"")</f>
+        <v/>
+      </c>
+      <c r="S62" s="11">
+        <f>IFERROR(AVERAGE(H62:P62),"")</f>
+        <v/>
+      </c>
+      <c r="T62" s="11">
+        <f>IFERROR(AVERAGE(E62:P62),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -3535,6 +3604,70 @@
           <t>Gas Differential (%)</t>
         </is>
       </c>
+      <c r="E63" s="11">
+        <f>IFERROR(E55/E$2,"")</f>
+        <v/>
+      </c>
+      <c r="F63" s="11">
+        <f>IFERROR(F55/F$2,"")</f>
+        <v/>
+      </c>
+      <c r="G63" s="11">
+        <f>IFERROR(G55/G$2,"")</f>
+        <v/>
+      </c>
+      <c r="H63" s="11">
+        <f>IFERROR(H55/H$2,"")</f>
+        <v/>
+      </c>
+      <c r="I63" s="11">
+        <f>IFERROR(I55/I$2,"")</f>
+        <v/>
+      </c>
+      <c r="J63" s="11">
+        <f>IFERROR(J55/J$2,"")</f>
+        <v/>
+      </c>
+      <c r="K63" s="11">
+        <f>IFERROR(K55/K$2,"")</f>
+        <v/>
+      </c>
+      <c r="L63" s="11">
+        <f>IFERROR(L55/L$2,"")</f>
+        <v/>
+      </c>
+      <c r="M63" s="11">
+        <f>IFERROR(M55/M$2,"")</f>
+        <v/>
+      </c>
+      <c r="N63" s="11">
+        <f>IFERROR(N55/N$2,"")</f>
+        <v/>
+      </c>
+      <c r="O63" s="11">
+        <f>IFERROR(O55/O$2,"")</f>
+        <v/>
+      </c>
+      <c r="P63" s="11">
+        <f>IFERROR(P55/P$2,"")</f>
+        <v/>
+      </c>
+      <c r="Q63" s="11">
+        <f>IFERROR(AVERAGE(N63:P63),"")</f>
+        <v/>
+      </c>
+      <c r="R63" s="11">
+        <f>IFERROR(AVERAGE(K63:P63),"")</f>
+        <v/>
+      </c>
+      <c r="S63" s="11">
+        <f>IFERROR(AVERAGE(H63:P63),"")</f>
+        <v/>
+      </c>
+      <c r="T63" s="11">
+        <f>IFERROR(AVERAGE(E63:P63),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -3550,6 +3683,70 @@
           <t>NGL Differential (%)</t>
         </is>
       </c>
+      <c r="E64" s="11">
+        <f>IFERROR(E56/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F64" s="11">
+        <f>IFERROR(F56/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G64" s="11">
+        <f>IFERROR(G56/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H64" s="11">
+        <f>IFERROR(H56/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I64" s="11">
+        <f>IFERROR(I56/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J64" s="11">
+        <f>IFERROR(J56/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K64" s="11">
+        <f>IFERROR(K56/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L64" s="11">
+        <f>IFERROR(L56/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M64" s="11">
+        <f>IFERROR(M56/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N64" s="11">
+        <f>IFERROR(N56/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O64" s="11">
+        <f>IFERROR(O56/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P64" s="11">
+        <f>IFERROR(P56/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q64" s="11">
+        <f>IFERROR(AVERAGE(N64:P64),"")</f>
+        <v/>
+      </c>
+      <c r="R64" s="11">
+        <f>IFERROR(AVERAGE(K64:P64),"")</f>
+        <v/>
+      </c>
+      <c r="S64" s="11">
+        <f>IFERROR(AVERAGE(H64:P64),"")</f>
+        <v/>
+      </c>
+      <c r="T64" s="11">
+        <f>IFERROR(AVERAGE(E64:P64),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -3575,6 +3772,54 @@
           <t>Gross Historical Gas Production (mcf)</t>
         </is>
       </c>
+      <c r="E66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;E$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="F66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;F$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="G66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;G$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="H66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;H$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;I$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="J66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;J$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="K66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;K$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="L66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;L$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="M66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;M$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="N66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;N$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="O66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;O$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="P66" s="12">
+        <f>+VLOOKUP($A66&amp;"-"&amp;P$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -3590,6 +3835,70 @@
           <t>Shrink (% remaining)</t>
         </is>
       </c>
+      <c r="E67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",E5:E48)/E66,"")</f>
+        <v/>
+      </c>
+      <c r="F67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",F5:F48)/F66,"")</f>
+        <v/>
+      </c>
+      <c r="G67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",G5:G48)/G66,"")</f>
+        <v/>
+      </c>
+      <c r="H67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",H5:H48)/H66,"")</f>
+        <v/>
+      </c>
+      <c r="I67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",I5:I48)/I66,"")</f>
+        <v/>
+      </c>
+      <c r="J67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",J5:J48)/J66,"")</f>
+        <v/>
+      </c>
+      <c r="K67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",K5:K48)/K66,"")</f>
+        <v/>
+      </c>
+      <c r="L67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",L5:L48)/L66,"")</f>
+        <v/>
+      </c>
+      <c r="M67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",M5:M48)/M66,"")</f>
+        <v/>
+      </c>
+      <c r="N67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",N5:N48)/N66,"")</f>
+        <v/>
+      </c>
+      <c r="O67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",O5:O48)/O66,"")</f>
+        <v/>
+      </c>
+      <c r="P67" s="11">
+        <f>IFERROR(SUMIF($D5:$D48,"Gas Sales Volumes (mcf)",P5:P48)/P66,"")</f>
+        <v/>
+      </c>
+      <c r="Q67" s="11">
+        <f>IFERROR(AVERAGE(N67:P67),"")</f>
+        <v/>
+      </c>
+      <c r="R67" s="11">
+        <f>IFERROR(AVERAGE(K67:P67),"")</f>
+        <v/>
+      </c>
+      <c r="S67" s="11">
+        <f>IFERROR(AVERAGE(H67:P67),"")</f>
+        <v/>
+      </c>
+      <c r="T67" s="11">
+        <f>IFERROR(AVERAGE(E67:P67),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -6766,6 +7075,70 @@
           <t>Oil Differential (%)</t>
         </is>
       </c>
+      <c r="E147" s="11">
+        <f>IFERROR(E139/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F147" s="11">
+        <f>IFERROR(F139/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G147" s="11">
+        <f>IFERROR(G139/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H147" s="11">
+        <f>IFERROR(H139/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I147" s="11">
+        <f>IFERROR(I139/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J147" s="11">
+        <f>IFERROR(J139/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K147" s="11">
+        <f>IFERROR(K139/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L147" s="11">
+        <f>IFERROR(L139/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M147" s="11">
+        <f>IFERROR(M139/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N147" s="11">
+        <f>IFERROR(N139/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O147" s="11">
+        <f>IFERROR(O139/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P147" s="11">
+        <f>IFERROR(P139/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q147" s="11">
+        <f>IFERROR(AVERAGE(N147:P147),"")</f>
+        <v/>
+      </c>
+      <c r="R147" s="11">
+        <f>IFERROR(AVERAGE(K147:P147),"")</f>
+        <v/>
+      </c>
+      <c r="S147" s="11">
+        <f>IFERROR(AVERAGE(H147:P147),"")</f>
+        <v/>
+      </c>
+      <c r="T147" s="11">
+        <f>IFERROR(AVERAGE(E147:P147),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="148">
       <c r="A148">
@@ -6781,6 +7154,70 @@
           <t>Gas Differential (%)</t>
         </is>
       </c>
+      <c r="E148" s="11">
+        <f>IFERROR(E140/E$2,"")</f>
+        <v/>
+      </c>
+      <c r="F148" s="11">
+        <f>IFERROR(F140/F$2,"")</f>
+        <v/>
+      </c>
+      <c r="G148" s="11">
+        <f>IFERROR(G140/G$2,"")</f>
+        <v/>
+      </c>
+      <c r="H148" s="11">
+        <f>IFERROR(H140/H$2,"")</f>
+        <v/>
+      </c>
+      <c r="I148" s="11">
+        <f>IFERROR(I140/I$2,"")</f>
+        <v/>
+      </c>
+      <c r="J148" s="11">
+        <f>IFERROR(J140/J$2,"")</f>
+        <v/>
+      </c>
+      <c r="K148" s="11">
+        <f>IFERROR(K140/K$2,"")</f>
+        <v/>
+      </c>
+      <c r="L148" s="11">
+        <f>IFERROR(L140/L$2,"")</f>
+        <v/>
+      </c>
+      <c r="M148" s="11">
+        <f>IFERROR(M140/M$2,"")</f>
+        <v/>
+      </c>
+      <c r="N148" s="11">
+        <f>IFERROR(N140/N$2,"")</f>
+        <v/>
+      </c>
+      <c r="O148" s="11">
+        <f>IFERROR(O140/O$2,"")</f>
+        <v/>
+      </c>
+      <c r="P148" s="11">
+        <f>IFERROR(P140/P$2,"")</f>
+        <v/>
+      </c>
+      <c r="Q148" s="11">
+        <f>IFERROR(AVERAGE(N148:P148),"")</f>
+        <v/>
+      </c>
+      <c r="R148" s="11">
+        <f>IFERROR(AVERAGE(K148:P148),"")</f>
+        <v/>
+      </c>
+      <c r="S148" s="11">
+        <f>IFERROR(AVERAGE(H148:P148),"")</f>
+        <v/>
+      </c>
+      <c r="T148" s="11">
+        <f>IFERROR(AVERAGE(E148:P148),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="149">
       <c r="A149">
@@ -6796,6 +7233,70 @@
           <t>NGL Differential (%)</t>
         </is>
       </c>
+      <c r="E149" s="11">
+        <f>IFERROR(E141/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F149" s="11">
+        <f>IFERROR(F141/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G149" s="11">
+        <f>IFERROR(G141/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H149" s="11">
+        <f>IFERROR(H141/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I149" s="11">
+        <f>IFERROR(I141/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J149" s="11">
+        <f>IFERROR(J141/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K149" s="11">
+        <f>IFERROR(K141/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L149" s="11">
+        <f>IFERROR(L141/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M149" s="11">
+        <f>IFERROR(M141/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N149" s="11">
+        <f>IFERROR(N141/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O149" s="11">
+        <f>IFERROR(O141/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P149" s="11">
+        <f>IFERROR(P141/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q149" s="11">
+        <f>IFERROR(AVERAGE(N149:P149),"")</f>
+        <v/>
+      </c>
+      <c r="R149" s="11">
+        <f>IFERROR(AVERAGE(K149:P149),"")</f>
+        <v/>
+      </c>
+      <c r="S149" s="11">
+        <f>IFERROR(AVERAGE(H149:P149),"")</f>
+        <v/>
+      </c>
+      <c r="T149" s="11">
+        <f>IFERROR(AVERAGE(E149:P149),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="150">
       <c r="A150">
@@ -6821,6 +7322,54 @@
           <t>Gross Historical Gas Production (mcf)</t>
         </is>
       </c>
+      <c r="E151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;E$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="F151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;F$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="G151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;G$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="H151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;H$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;I$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="J151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;J$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="K151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;K$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="L151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;L$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="M151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;M$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="N151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;N$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="O151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;O$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="P151" s="12">
+        <f>+VLOOKUP($A151&amp;"-"&amp;P$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
     </row>
     <row r="152">
       <c r="A152">
@@ -6836,6 +7385,70 @@
           <t>Shrink (% remaining)</t>
         </is>
       </c>
+      <c r="E152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",E90:E133)/E151,"")</f>
+        <v/>
+      </c>
+      <c r="F152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",F90:F133)/F151,"")</f>
+        <v/>
+      </c>
+      <c r="G152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",G90:G133)/G151,"")</f>
+        <v/>
+      </c>
+      <c r="H152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",H90:H133)/H151,"")</f>
+        <v/>
+      </c>
+      <c r="I152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",I90:I133)/I151,"")</f>
+        <v/>
+      </c>
+      <c r="J152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",J90:J133)/J151,"")</f>
+        <v/>
+      </c>
+      <c r="K152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",K90:K133)/K151,"")</f>
+        <v/>
+      </c>
+      <c r="L152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",L90:L133)/L151,"")</f>
+        <v/>
+      </c>
+      <c r="M152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",M90:M133)/M151,"")</f>
+        <v/>
+      </c>
+      <c r="N152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",N90:N133)/N151,"")</f>
+        <v/>
+      </c>
+      <c r="O152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",O90:O133)/O151,"")</f>
+        <v/>
+      </c>
+      <c r="P152" s="11">
+        <f>IFERROR(SUMIF($D90:$D133,"Gas Sales Volumes (mcf)",P90:P133)/P151,"")</f>
+        <v/>
+      </c>
+      <c r="Q152" s="11">
+        <f>IFERROR(AVERAGE(N152:P152),"")</f>
+        <v/>
+      </c>
+      <c r="R152" s="11">
+        <f>IFERROR(AVERAGE(K152:P152),"")</f>
+        <v/>
+      </c>
+      <c r="S152" s="11">
+        <f>IFERROR(AVERAGE(H152:P152),"")</f>
+        <v/>
+      </c>
+      <c r="T152" s="11">
+        <f>IFERROR(AVERAGE(E152:P152),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="153">
       <c r="A153">
@@ -10012,6 +10625,70 @@
           <t>Oil Differential (%)</t>
         </is>
       </c>
+      <c r="E232" s="11">
+        <f>IFERROR(E224/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F232" s="11">
+        <f>IFERROR(F224/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G232" s="11">
+        <f>IFERROR(G224/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H232" s="11">
+        <f>IFERROR(H224/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I232" s="11">
+        <f>IFERROR(I224/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J232" s="11">
+        <f>IFERROR(J224/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K232" s="11">
+        <f>IFERROR(K224/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L232" s="11">
+        <f>IFERROR(L224/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M232" s="11">
+        <f>IFERROR(M224/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N232" s="11">
+        <f>IFERROR(N224/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O232" s="11">
+        <f>IFERROR(O224/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P232" s="11">
+        <f>IFERROR(P224/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q232" s="11">
+        <f>IFERROR(AVERAGE(N232:P232),"")</f>
+        <v/>
+      </c>
+      <c r="R232" s="11">
+        <f>IFERROR(AVERAGE(K232:P232),"")</f>
+        <v/>
+      </c>
+      <c r="S232" s="11">
+        <f>IFERROR(AVERAGE(H232:P232),"")</f>
+        <v/>
+      </c>
+      <c r="T232" s="11">
+        <f>IFERROR(AVERAGE(E232:P232),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -10027,6 +10704,70 @@
           <t>Gas Differential (%)</t>
         </is>
       </c>
+      <c r="E233" s="11">
+        <f>IFERROR(E225/E$2,"")</f>
+        <v/>
+      </c>
+      <c r="F233" s="11">
+        <f>IFERROR(F225/F$2,"")</f>
+        <v/>
+      </c>
+      <c r="G233" s="11">
+        <f>IFERROR(G225/G$2,"")</f>
+        <v/>
+      </c>
+      <c r="H233" s="11">
+        <f>IFERROR(H225/H$2,"")</f>
+        <v/>
+      </c>
+      <c r="I233" s="11">
+        <f>IFERROR(I225/I$2,"")</f>
+        <v/>
+      </c>
+      <c r="J233" s="11">
+        <f>IFERROR(J225/J$2,"")</f>
+        <v/>
+      </c>
+      <c r="K233" s="11">
+        <f>IFERROR(K225/K$2,"")</f>
+        <v/>
+      </c>
+      <c r="L233" s="11">
+        <f>IFERROR(L225/L$2,"")</f>
+        <v/>
+      </c>
+      <c r="M233" s="11">
+        <f>IFERROR(M225/M$2,"")</f>
+        <v/>
+      </c>
+      <c r="N233" s="11">
+        <f>IFERROR(N225/N$2,"")</f>
+        <v/>
+      </c>
+      <c r="O233" s="11">
+        <f>IFERROR(O225/O$2,"")</f>
+        <v/>
+      </c>
+      <c r="P233" s="11">
+        <f>IFERROR(P225/P$2,"")</f>
+        <v/>
+      </c>
+      <c r="Q233" s="11">
+        <f>IFERROR(AVERAGE(N233:P233),"")</f>
+        <v/>
+      </c>
+      <c r="R233" s="11">
+        <f>IFERROR(AVERAGE(K233:P233),"")</f>
+        <v/>
+      </c>
+      <c r="S233" s="11">
+        <f>IFERROR(AVERAGE(H233:P233),"")</f>
+        <v/>
+      </c>
+      <c r="T233" s="11">
+        <f>IFERROR(AVERAGE(E233:P233),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -10042,6 +10783,70 @@
           <t>NGL Differential (%)</t>
         </is>
       </c>
+      <c r="E234" s="11">
+        <f>IFERROR(E226/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F234" s="11">
+        <f>IFERROR(F226/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G234" s="11">
+        <f>IFERROR(G226/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H234" s="11">
+        <f>IFERROR(H226/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I234" s="11">
+        <f>IFERROR(I226/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J234" s="11">
+        <f>IFERROR(J226/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K234" s="11">
+        <f>IFERROR(K226/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L234" s="11">
+        <f>IFERROR(L226/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M234" s="11">
+        <f>IFERROR(M226/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N234" s="11">
+        <f>IFERROR(N226/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O234" s="11">
+        <f>IFERROR(O226/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P234" s="11">
+        <f>IFERROR(P226/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q234" s="11">
+        <f>IFERROR(AVERAGE(N234:P234),"")</f>
+        <v/>
+      </c>
+      <c r="R234" s="11">
+        <f>IFERROR(AVERAGE(K234:P234),"")</f>
+        <v/>
+      </c>
+      <c r="S234" s="11">
+        <f>IFERROR(AVERAGE(H234:P234),"")</f>
+        <v/>
+      </c>
+      <c r="T234" s="11">
+        <f>IFERROR(AVERAGE(E234:P234),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -10067,6 +10872,54 @@
           <t>Gross Historical Gas Production (mcf)</t>
         </is>
       </c>
+      <c r="E236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;E$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="F236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;F$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="G236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;G$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="H236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;H$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;I$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="J236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;J$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="K236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;K$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="L236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;L$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="M236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;M$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="N236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;N$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="O236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;O$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="P236" s="12">
+        <f>+VLOOKUP($A236&amp;"-"&amp;P$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -10082,6 +10935,70 @@
           <t>Shrink (% remaining)</t>
         </is>
       </c>
+      <c r="E237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",E175:E218)/E236,"")</f>
+        <v/>
+      </c>
+      <c r="F237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",F175:F218)/F236,"")</f>
+        <v/>
+      </c>
+      <c r="G237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",G175:G218)/G236,"")</f>
+        <v/>
+      </c>
+      <c r="H237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",H175:H218)/H236,"")</f>
+        <v/>
+      </c>
+      <c r="I237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",I175:I218)/I236,"")</f>
+        <v/>
+      </c>
+      <c r="J237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",J175:J218)/J236,"")</f>
+        <v/>
+      </c>
+      <c r="K237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",K175:K218)/K236,"")</f>
+        <v/>
+      </c>
+      <c r="L237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",L175:L218)/L236,"")</f>
+        <v/>
+      </c>
+      <c r="M237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",M175:M218)/M236,"")</f>
+        <v/>
+      </c>
+      <c r="N237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",N175:N218)/N236,"")</f>
+        <v/>
+      </c>
+      <c r="O237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",O175:O218)/O236,"")</f>
+        <v/>
+      </c>
+      <c r="P237" s="11">
+        <f>IFERROR(SUMIF($D175:$D218,"Gas Sales Volumes (mcf)",P175:P218)/P236,"")</f>
+        <v/>
+      </c>
+      <c r="Q237" s="11">
+        <f>IFERROR(AVERAGE(N237:P237),"")</f>
+        <v/>
+      </c>
+      <c r="R237" s="11">
+        <f>IFERROR(AVERAGE(K237:P237),"")</f>
+        <v/>
+      </c>
+      <c r="S237" s="11">
+        <f>IFERROR(AVERAGE(H237:P237),"")</f>
+        <v/>
+      </c>
+      <c r="T237" s="11">
+        <f>IFERROR(AVERAGE(E237:P237),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -13258,6 +14175,70 @@
           <t>Oil Differential (%)</t>
         </is>
       </c>
+      <c r="E317" s="11">
+        <f>IFERROR(E309/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F317" s="11">
+        <f>IFERROR(F309/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G317" s="11">
+        <f>IFERROR(G309/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H317" s="11">
+        <f>IFERROR(H309/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I317" s="11">
+        <f>IFERROR(I309/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J317" s="11">
+        <f>IFERROR(J309/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K317" s="11">
+        <f>IFERROR(K309/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L317" s="11">
+        <f>IFERROR(L309/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M317" s="11">
+        <f>IFERROR(M309/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N317" s="11">
+        <f>IFERROR(N309/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O317" s="11">
+        <f>IFERROR(O309/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P317" s="11">
+        <f>IFERROR(P309/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q317" s="11">
+        <f>IFERROR(AVERAGE(N317:P317),"")</f>
+        <v/>
+      </c>
+      <c r="R317" s="11">
+        <f>IFERROR(AVERAGE(K317:P317),"")</f>
+        <v/>
+      </c>
+      <c r="S317" s="11">
+        <f>IFERROR(AVERAGE(H317:P317),"")</f>
+        <v/>
+      </c>
+      <c r="T317" s="11">
+        <f>IFERROR(AVERAGE(E317:P317),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="318">
       <c r="A318">
@@ -13273,6 +14254,70 @@
           <t>Gas Differential (%)</t>
         </is>
       </c>
+      <c r="E318" s="11">
+        <f>IFERROR(E310/E$2,"")</f>
+        <v/>
+      </c>
+      <c r="F318" s="11">
+        <f>IFERROR(F310/F$2,"")</f>
+        <v/>
+      </c>
+      <c r="G318" s="11">
+        <f>IFERROR(G310/G$2,"")</f>
+        <v/>
+      </c>
+      <c r="H318" s="11">
+        <f>IFERROR(H310/H$2,"")</f>
+        <v/>
+      </c>
+      <c r="I318" s="11">
+        <f>IFERROR(I310/I$2,"")</f>
+        <v/>
+      </c>
+      <c r="J318" s="11">
+        <f>IFERROR(J310/J$2,"")</f>
+        <v/>
+      </c>
+      <c r="K318" s="11">
+        <f>IFERROR(K310/K$2,"")</f>
+        <v/>
+      </c>
+      <c r="L318" s="11">
+        <f>IFERROR(L310/L$2,"")</f>
+        <v/>
+      </c>
+      <c r="M318" s="11">
+        <f>IFERROR(M310/M$2,"")</f>
+        <v/>
+      </c>
+      <c r="N318" s="11">
+        <f>IFERROR(N310/N$2,"")</f>
+        <v/>
+      </c>
+      <c r="O318" s="11">
+        <f>IFERROR(O310/O$2,"")</f>
+        <v/>
+      </c>
+      <c r="P318" s="11">
+        <f>IFERROR(P310/P$2,"")</f>
+        <v/>
+      </c>
+      <c r="Q318" s="11">
+        <f>IFERROR(AVERAGE(N318:P318),"")</f>
+        <v/>
+      </c>
+      <c r="R318" s="11">
+        <f>IFERROR(AVERAGE(K318:P318),"")</f>
+        <v/>
+      </c>
+      <c r="S318" s="11">
+        <f>IFERROR(AVERAGE(H318:P318),"")</f>
+        <v/>
+      </c>
+      <c r="T318" s="11">
+        <f>IFERROR(AVERAGE(E318:P318),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="319">
       <c r="A319">
@@ -13288,6 +14333,70 @@
           <t>NGL Differential (%)</t>
         </is>
       </c>
+      <c r="E319" s="11">
+        <f>IFERROR(E311/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F319" s="11">
+        <f>IFERROR(F311/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G319" s="11">
+        <f>IFERROR(G311/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H319" s="11">
+        <f>IFERROR(H311/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I319" s="11">
+        <f>IFERROR(I311/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J319" s="11">
+        <f>IFERROR(J311/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K319" s="11">
+        <f>IFERROR(K311/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L319" s="11">
+        <f>IFERROR(L311/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M319" s="11">
+        <f>IFERROR(M311/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N319" s="11">
+        <f>IFERROR(N311/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O319" s="11">
+        <f>IFERROR(O311/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P319" s="11">
+        <f>IFERROR(P311/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q319" s="11">
+        <f>IFERROR(AVERAGE(N319:P319),"")</f>
+        <v/>
+      </c>
+      <c r="R319" s="11">
+        <f>IFERROR(AVERAGE(K319:P319),"")</f>
+        <v/>
+      </c>
+      <c r="S319" s="11">
+        <f>IFERROR(AVERAGE(H319:P319),"")</f>
+        <v/>
+      </c>
+      <c r="T319" s="11">
+        <f>IFERROR(AVERAGE(E319:P319),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="320">
       <c r="A320">
@@ -13313,6 +14422,54 @@
           <t>Gross Historical Gas Production (mcf)</t>
         </is>
       </c>
+      <c r="E321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;E$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="F321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;F$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="G321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;G$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="H321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;H$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;I$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="J321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;J$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="K321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;K$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="L321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;L$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="M321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;M$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="N321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;N$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="O321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;O$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="P321" s="12">
+        <f>+VLOOKUP($A321&amp;"-"&amp;P$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
     </row>
     <row r="322">
       <c r="A322">
@@ -13328,6 +14485,70 @@
           <t>Shrink (% remaining)</t>
         </is>
       </c>
+      <c r="E322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",E260:E303)/E321,"")</f>
+        <v/>
+      </c>
+      <c r="F322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",F260:F303)/F321,"")</f>
+        <v/>
+      </c>
+      <c r="G322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",G260:G303)/G321,"")</f>
+        <v/>
+      </c>
+      <c r="H322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",H260:H303)/H321,"")</f>
+        <v/>
+      </c>
+      <c r="I322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",I260:I303)/I321,"")</f>
+        <v/>
+      </c>
+      <c r="J322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",J260:J303)/J321,"")</f>
+        <v/>
+      </c>
+      <c r="K322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",K260:K303)/K321,"")</f>
+        <v/>
+      </c>
+      <c r="L322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",L260:L303)/L321,"")</f>
+        <v/>
+      </c>
+      <c r="M322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",M260:M303)/M321,"")</f>
+        <v/>
+      </c>
+      <c r="N322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",N260:N303)/N321,"")</f>
+        <v/>
+      </c>
+      <c r="O322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",O260:O303)/O321,"")</f>
+        <v/>
+      </c>
+      <c r="P322" s="11">
+        <f>IFERROR(SUMIF($D260:$D303,"Gas Sales Volumes (mcf)",P260:P303)/P321,"")</f>
+        <v/>
+      </c>
+      <c r="Q322" s="11">
+        <f>IFERROR(AVERAGE(N322:P322),"")</f>
+        <v/>
+      </c>
+      <c r="R322" s="11">
+        <f>IFERROR(AVERAGE(K322:P322),"")</f>
+        <v/>
+      </c>
+      <c r="S322" s="11">
+        <f>IFERROR(AVERAGE(H322:P322),"")</f>
+        <v/>
+      </c>
+      <c r="T322" s="11">
+        <f>IFERROR(AVERAGE(E322:P322),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="323">
       <c r="A323">
@@ -16504,6 +17725,70 @@
           <t>Oil Differential (%)</t>
         </is>
       </c>
+      <c r="E402" s="11">
+        <f>IFERROR(E394/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F402" s="11">
+        <f>IFERROR(F394/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G402" s="11">
+        <f>IFERROR(G394/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H402" s="11">
+        <f>IFERROR(H394/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I402" s="11">
+        <f>IFERROR(I394/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J402" s="11">
+        <f>IFERROR(J394/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K402" s="11">
+        <f>IFERROR(K394/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L402" s="11">
+        <f>IFERROR(L394/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M402" s="11">
+        <f>IFERROR(M394/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N402" s="11">
+        <f>IFERROR(N394/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O402" s="11">
+        <f>IFERROR(O394/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P402" s="11">
+        <f>IFERROR(P394/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q402" s="11">
+        <f>IFERROR(AVERAGE(N402:P402),"")</f>
+        <v/>
+      </c>
+      <c r="R402" s="11">
+        <f>IFERROR(AVERAGE(K402:P402),"")</f>
+        <v/>
+      </c>
+      <c r="S402" s="11">
+        <f>IFERROR(AVERAGE(H402:P402),"")</f>
+        <v/>
+      </c>
+      <c r="T402" s="11">
+        <f>IFERROR(AVERAGE(E402:P402),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="403">
       <c r="A403">
@@ -16519,6 +17804,70 @@
           <t>Gas Differential (%)</t>
         </is>
       </c>
+      <c r="E403" s="11">
+        <f>IFERROR(E395/E$2,"")</f>
+        <v/>
+      </c>
+      <c r="F403" s="11">
+        <f>IFERROR(F395/F$2,"")</f>
+        <v/>
+      </c>
+      <c r="G403" s="11">
+        <f>IFERROR(G395/G$2,"")</f>
+        <v/>
+      </c>
+      <c r="H403" s="11">
+        <f>IFERROR(H395/H$2,"")</f>
+        <v/>
+      </c>
+      <c r="I403" s="11">
+        <f>IFERROR(I395/I$2,"")</f>
+        <v/>
+      </c>
+      <c r="J403" s="11">
+        <f>IFERROR(J395/J$2,"")</f>
+        <v/>
+      </c>
+      <c r="K403" s="11">
+        <f>IFERROR(K395/K$2,"")</f>
+        <v/>
+      </c>
+      <c r="L403" s="11">
+        <f>IFERROR(L395/L$2,"")</f>
+        <v/>
+      </c>
+      <c r="M403" s="11">
+        <f>IFERROR(M395/M$2,"")</f>
+        <v/>
+      </c>
+      <c r="N403" s="11">
+        <f>IFERROR(N395/N$2,"")</f>
+        <v/>
+      </c>
+      <c r="O403" s="11">
+        <f>IFERROR(O395/O$2,"")</f>
+        <v/>
+      </c>
+      <c r="P403" s="11">
+        <f>IFERROR(P395/P$2,"")</f>
+        <v/>
+      </c>
+      <c r="Q403" s="11">
+        <f>IFERROR(AVERAGE(N403:P403),"")</f>
+        <v/>
+      </c>
+      <c r="R403" s="11">
+        <f>IFERROR(AVERAGE(K403:P403),"")</f>
+        <v/>
+      </c>
+      <c r="S403" s="11">
+        <f>IFERROR(AVERAGE(H403:P403),"")</f>
+        <v/>
+      </c>
+      <c r="T403" s="11">
+        <f>IFERROR(AVERAGE(E403:P403),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="404">
       <c r="A404">
@@ -16534,6 +17883,70 @@
           <t>NGL Differential (%)</t>
         </is>
       </c>
+      <c r="E404" s="11">
+        <f>IFERROR(E396/E$1,"")</f>
+        <v/>
+      </c>
+      <c r="F404" s="11">
+        <f>IFERROR(F396/F$1,"")</f>
+        <v/>
+      </c>
+      <c r="G404" s="11">
+        <f>IFERROR(G396/G$1,"")</f>
+        <v/>
+      </c>
+      <c r="H404" s="11">
+        <f>IFERROR(H396/H$1,"")</f>
+        <v/>
+      </c>
+      <c r="I404" s="11">
+        <f>IFERROR(I396/I$1,"")</f>
+        <v/>
+      </c>
+      <c r="J404" s="11">
+        <f>IFERROR(J396/J$1,"")</f>
+        <v/>
+      </c>
+      <c r="K404" s="11">
+        <f>IFERROR(K396/K$1,"")</f>
+        <v/>
+      </c>
+      <c r="L404" s="11">
+        <f>IFERROR(L396/L$1,"")</f>
+        <v/>
+      </c>
+      <c r="M404" s="11">
+        <f>IFERROR(M396/M$1,"")</f>
+        <v/>
+      </c>
+      <c r="N404" s="11">
+        <f>IFERROR(N396/N$1,"")</f>
+        <v/>
+      </c>
+      <c r="O404" s="11">
+        <f>IFERROR(O396/O$1,"")</f>
+        <v/>
+      </c>
+      <c r="P404" s="11">
+        <f>IFERROR(P396/P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q404" s="11">
+        <f>IFERROR(AVERAGE(N404:P404),"")</f>
+        <v/>
+      </c>
+      <c r="R404" s="11">
+        <f>IFERROR(AVERAGE(K404:P404),"")</f>
+        <v/>
+      </c>
+      <c r="S404" s="11">
+        <f>IFERROR(AVERAGE(H404:P404),"")</f>
+        <v/>
+      </c>
+      <c r="T404" s="11">
+        <f>IFERROR(AVERAGE(E404:P404),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="405">
       <c r="A405">
@@ -16559,6 +17972,54 @@
           <t>Gross Historical Gas Production (mcf)</t>
         </is>
       </c>
+      <c r="E406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;E$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="F406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;F$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="G406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;G$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="H406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;H$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="I406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;I$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="J406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;J$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="K406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;K$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="L406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;L$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="M406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;M$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="N406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;N$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="O406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;O$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
+      <c r="P406" s="12">
+        <f>+VLOOKUP($A406&amp;"-"&amp;P$4,Example0gross_HistoricalProd!$A:$E,5,FALSE)</f>
+        <v/>
+      </c>
     </row>
     <row r="407">
       <c r="A407">
@@ -16573,6 +18034,70 @@
         <is>
           <t>Shrink (% remaining)</t>
         </is>
+      </c>
+      <c r="E407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",E345:E388)/E406,"")</f>
+        <v/>
+      </c>
+      <c r="F407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",F345:F388)/F406,"")</f>
+        <v/>
+      </c>
+      <c r="G407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",G345:G388)/G406,"")</f>
+        <v/>
+      </c>
+      <c r="H407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",H345:H388)/H406,"")</f>
+        <v/>
+      </c>
+      <c r="I407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",I345:I388)/I406,"")</f>
+        <v/>
+      </c>
+      <c r="J407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",J345:J388)/J406,"")</f>
+        <v/>
+      </c>
+      <c r="K407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",K345:K388)/K406,"")</f>
+        <v/>
+      </c>
+      <c r="L407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",L345:L388)/L406,"")</f>
+        <v/>
+      </c>
+      <c r="M407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",M345:M388)/M406,"")</f>
+        <v/>
+      </c>
+      <c r="N407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",N345:N388)/N406,"")</f>
+        <v/>
+      </c>
+      <c r="O407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",O345:O388)/O406,"")</f>
+        <v/>
+      </c>
+      <c r="P407" s="11">
+        <f>IFERROR(SUMIF($D345:$D388,"Gas Sales Volumes (mcf)",P345:P388)/P406,"")</f>
+        <v/>
+      </c>
+      <c r="Q407" s="11">
+        <f>IFERROR(AVERAGE(N407:P407),"")</f>
+        <v/>
+      </c>
+      <c r="R407" s="11">
+        <f>IFERROR(AVERAGE(K407:P407),"")</f>
+        <v/>
+      </c>
+      <c r="S407" s="11">
+        <f>IFERROR(AVERAGE(H407:P407),"")</f>
+        <v/>
+      </c>
+      <c r="T407" s="11">
+        <f>IFERROR(AVERAGE(E407:P407),"")</f>
+        <v/>
       </c>
     </row>
     <row r="408">
@@ -18694,7 +20219,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -18706,1657 +20231,1782 @@
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
         <is>
+          <t>Composite Key</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
           <t>Case Name</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>PHDWIN Id</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Historical Gas Production</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Historical Oil Production</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Historical Water Production</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Historical Well Count</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2">
+        <f>+C2&amp;"-"&amp;D2</f>
+        <v/>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>103</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Jan-23</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="D2" s="13" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E2" t="n">
         <v>8250</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1200</v>
       </c>
       <c r="F2" t="n">
         <v>1200</v>
       </c>
       <c r="G2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3">
+        <f>+C3&amp;"-"&amp;D3</f>
+        <v/>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>103</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Feb-23</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+      <c r="D3" s="13" t="n">
+        <v>44958</v>
+      </c>
+      <c r="E3" t="n">
         <v>8456</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1230</v>
       </c>
       <c r="F3" t="n">
         <v>1230</v>
       </c>
       <c r="G3" t="n">
+        <v>1230</v>
+      </c>
+      <c r="H3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4">
+        <f>+C4&amp;"-"&amp;D4</f>
+        <v/>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>103</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Mar-23</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="D4" s="13" t="n">
+        <v>44986</v>
+      </c>
+      <c r="E4" t="n">
         <v>8668</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1260.75</v>
       </c>
       <c r="F4" t="n">
         <v>1260.75</v>
       </c>
       <c r="G4" t="n">
+        <v>1260.75</v>
+      </c>
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5">
+        <f>+C5&amp;"-"&amp;D5</f>
+        <v/>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>103</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Apr-23</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="D5" s="13" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E5" t="n">
         <v>8884</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1292.26875</v>
       </c>
       <c r="F5" t="n">
         <v>1292.26875</v>
       </c>
       <c r="G5" t="n">
+        <v>1292.26875</v>
+      </c>
+      <c r="H5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6">
+        <f>+C6&amp;"-"&amp;D6</f>
+        <v/>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>103</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+      <c r="D6" s="13" t="n">
+        <v>45047</v>
+      </c>
+      <c r="E6" t="n">
         <v>9106</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1324.57546875</v>
       </c>
       <c r="F6" t="n">
         <v>1324.57546875</v>
       </c>
       <c r="G6" t="n">
+        <v>1324.57546875</v>
+      </c>
+      <c r="H6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7">
+        <f>+C7&amp;"-"&amp;D7</f>
+        <v/>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>103</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Jun-23</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="D7" s="13" t="n">
+        <v>45078</v>
+      </c>
+      <c r="E7" t="n">
         <v>9334</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1357.68985546875</v>
       </c>
       <c r="F7" t="n">
         <v>1357.68985546875</v>
       </c>
       <c r="G7" t="n">
+        <v>1357.68985546875</v>
+      </c>
+      <c r="H7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8">
+        <f>+C8&amp;"-"&amp;D8</f>
+        <v/>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>103</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Jul-23</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+      <c r="D8" s="13" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E8" t="n">
         <v>9567</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1391.632101855468</v>
       </c>
       <c r="F8" t="n">
         <v>1391.632101855468</v>
       </c>
       <c r="G8" t="n">
+        <v>1391.632101855468</v>
+      </c>
+      <c r="H8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9">
+        <f>+C9&amp;"-"&amp;D9</f>
+        <v/>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>103</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Aug-23</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="D9" s="13" t="n">
+        <v>45139</v>
+      </c>
+      <c r="E9" t="n">
         <v>9807</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1426.422904401855</v>
       </c>
       <c r="F9" t="n">
         <v>1426.422904401855</v>
       </c>
       <c r="G9" t="n">
+        <v>1426.422904401855</v>
+      </c>
+      <c r="H9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10">
+        <f>+C10&amp;"-"&amp;D10</f>
+        <v/>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>103</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Sep-23</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+      <c r="D10" s="13" t="n">
+        <v>45170</v>
+      </c>
+      <c r="E10" t="n">
         <v>10052</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1462.083477011901</v>
       </c>
       <c r="F10" t="n">
         <v>1462.083477011901</v>
       </c>
       <c r="G10" t="n">
+        <v>1462.083477011901</v>
+      </c>
+      <c r="H10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11">
+        <f>+C11&amp;"-"&amp;D11</f>
+        <v/>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>103</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Oct-23</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+      <c r="D11" s="13" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E11" t="n">
         <v>10303</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1498.635563937199</v>
       </c>
       <c r="F11" t="n">
         <v>1498.635563937199</v>
       </c>
       <c r="G11" t="n">
+        <v>1498.635563937199</v>
+      </c>
+      <c r="H11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12">
+        <f>+C12&amp;"-"&amp;D12</f>
+        <v/>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>103</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Nov-23</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
+      <c r="D12" s="13" t="n">
+        <v>45231</v>
+      </c>
+      <c r="E12" t="n">
         <v>10561</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1536.101453035629</v>
       </c>
       <c r="F12" t="n">
         <v>1536.101453035629</v>
       </c>
       <c r="G12" t="n">
+        <v>1536.101453035629</v>
+      </c>
+      <c r="H12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13">
+        <f>+C13&amp;"-"&amp;D13</f>
+        <v/>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Jimmy 1-H</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>103</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Dec-23</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
+      <c r="D13" s="13" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E13" t="n">
         <v>10825</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1574.503989361519</v>
       </c>
       <c r="F13" t="n">
         <v>1574.503989361519</v>
       </c>
       <c r="G13" t="n">
+        <v>1574.503989361519</v>
+      </c>
+      <c r="H13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14">
+        <f>+C14&amp;"-"&amp;D14</f>
+        <v/>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>104</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Jan-23</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
+      <c r="D14" s="13" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E14" t="n">
         <v>7838</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1140</v>
       </c>
       <c r="F14" t="n">
         <v>1140</v>
       </c>
       <c r="G14" t="n">
+        <v>1140</v>
+      </c>
+      <c r="H14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15">
+        <f>+C15&amp;"-"&amp;D15</f>
+        <v/>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>104</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Feb-23</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
+      <c r="D15" s="13" t="n">
+        <v>44958</v>
+      </c>
+      <c r="E15" t="n">
         <v>8033</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1168.5</v>
       </c>
       <c r="F15" t="n">
         <v>1168.5</v>
       </c>
       <c r="G15" t="n">
+        <v>1168.5</v>
+      </c>
+      <c r="H15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16">
+        <f>+C16&amp;"-"&amp;D16</f>
+        <v/>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>104</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Mar-23</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
+      <c r="D16" s="13" t="n">
+        <v>44986</v>
+      </c>
+      <c r="E16" t="n">
         <v>8234</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1197.7125</v>
       </c>
       <c r="F16" t="n">
         <v>1197.7125</v>
       </c>
       <c r="G16" t="n">
+        <v>1197.7125</v>
+      </c>
+      <c r="H16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17">
+        <f>+C17&amp;"-"&amp;D17</f>
+        <v/>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>104</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Apr-23</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
+      <c r="D17" s="13" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E17" t="n">
         <v>8440</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1227.6553125</v>
       </c>
       <c r="F17" t="n">
         <v>1227.6553125</v>
       </c>
       <c r="G17" t="n">
+        <v>1227.6553125</v>
+      </c>
+      <c r="H17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18">
+        <f>+C18&amp;"-"&amp;D18</f>
+        <v/>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>104</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+      <c r="D18" s="13" t="n">
+        <v>45047</v>
+      </c>
+      <c r="E18" t="n">
         <v>8651</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1258.3466953125</v>
       </c>
       <c r="F18" t="n">
         <v>1258.3466953125</v>
       </c>
       <c r="G18" t="n">
+        <v>1258.3466953125</v>
+      </c>
+      <c r="H18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19">
+        <f>+C19&amp;"-"&amp;D19</f>
+        <v/>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>104</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Jun-23</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
+      <c r="D19" s="13" t="n">
+        <v>45078</v>
+      </c>
+      <c r="E19" t="n">
         <v>8867</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1289.805362695312</v>
       </c>
       <c r="F19" t="n">
         <v>1289.805362695312</v>
       </c>
       <c r="G19" t="n">
+        <v>1289.805362695312</v>
+      </c>
+      <c r="H19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20">
+        <f>+C20&amp;"-"&amp;D20</f>
+        <v/>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>104</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Jul-23</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
+      <c r="D20" s="13" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E20" t="n">
         <v>9089</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1322.050496762695</v>
       </c>
       <c r="F20" t="n">
         <v>1322.050496762695</v>
       </c>
       <c r="G20" t="n">
+        <v>1322.050496762695</v>
+      </c>
+      <c r="H20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21">
+        <f>+C21&amp;"-"&amp;D21</f>
+        <v/>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="n">
         <v>104</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Aug-23</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
+      <c r="D21" s="13" t="n">
+        <v>45139</v>
+      </c>
+      <c r="E21" t="n">
         <v>9316</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1355.101759181762</v>
       </c>
       <c r="F21" t="n">
         <v>1355.101759181762</v>
       </c>
       <c r="G21" t="n">
+        <v>1355.101759181762</v>
+      </c>
+      <c r="H21" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22">
+        <f>+C22&amp;"-"&amp;D22</f>
+        <v/>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="n">
         <v>104</v>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Sep-23</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
+      <c r="D22" s="13" t="n">
+        <v>45170</v>
+      </c>
+      <c r="E22" t="n">
         <v>9549</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1388.979303161306</v>
       </c>
       <c r="F22" t="n">
         <v>1388.979303161306</v>
       </c>
       <c r="G22" t="n">
+        <v>1388.979303161306</v>
+      </c>
+      <c r="H22" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23">
+        <f>+C23&amp;"-"&amp;D23</f>
+        <v/>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="n">
         <v>104</v>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Oct-23</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
+      <c r="D23" s="13" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E23" t="n">
         <v>9788</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1423.703785740339</v>
       </c>
       <c r="F23" t="n">
         <v>1423.703785740339</v>
       </c>
       <c r="G23" t="n">
+        <v>1423.703785740339</v>
+      </c>
+      <c r="H23" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24">
+        <f>+C24&amp;"-"&amp;D24</f>
+        <v/>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="n">
         <v>104</v>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Nov-23</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
+      <c r="D24" s="13" t="n">
+        <v>45231</v>
+      </c>
+      <c r="E24" t="n">
         <v>10033</v>
-      </c>
-      <c r="E24" t="n">
-        <v>1459.296380383847</v>
       </c>
       <c r="F24" t="n">
         <v>1459.296380383847</v>
       </c>
       <c r="G24" t="n">
+        <v>1459.296380383847</v>
+      </c>
+      <c r="H24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25">
+        <f>+C25&amp;"-"&amp;D25</f>
+        <v/>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>Bobby 3-H</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="C25" t="n">
         <v>104</v>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Dec-23</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+      <c r="D25" s="13" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E25" t="n">
         <v>10283</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1495.778789893443</v>
       </c>
       <c r="F25" t="n">
         <v>1495.778789893443</v>
       </c>
       <c r="G25" t="n">
+        <v>1495.778789893443</v>
+      </c>
+      <c r="H25" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26">
+        <f>+C26&amp;"-"&amp;D26</f>
+        <v/>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="C26" t="n">
         <v>105</v>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Jan-23</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
+      <c r="D26" s="13" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E26" t="n">
         <v>6555</v>
-      </c>
-      <c r="E26" t="n">
-        <v>912</v>
       </c>
       <c r="F26" t="n">
         <v>912</v>
       </c>
       <c r="G26" t="n">
+        <v>912</v>
+      </c>
+      <c r="H26" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27">
+        <f>+C27&amp;"-"&amp;D27</f>
+        <v/>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="C27" t="n">
         <v>105</v>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Feb-23</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
+      <c r="D27" s="13" t="n">
+        <v>44958</v>
+      </c>
+      <c r="E27" t="n">
         <v>6719</v>
-      </c>
-      <c r="E27" t="n">
-        <v>934.8000000000001</v>
       </c>
       <c r="F27" t="n">
         <v>934.8000000000001</v>
       </c>
       <c r="G27" t="n">
+        <v>934.8000000000001</v>
+      </c>
+      <c r="H27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28">
+        <f>+C28&amp;"-"&amp;D28</f>
+        <v/>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="C28" t="n">
         <v>105</v>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Mar-23</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
+      <c r="D28" s="13" t="n">
+        <v>44986</v>
+      </c>
+      <c r="E28" t="n">
         <v>6887</v>
-      </c>
-      <c r="E28" t="n">
-        <v>958.17</v>
       </c>
       <c r="F28" t="n">
         <v>958.17</v>
       </c>
       <c r="G28" t="n">
+        <v>958.17</v>
+      </c>
+      <c r="H28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29">
+        <f>+C29&amp;"-"&amp;D29</f>
+        <v/>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="C29" t="n">
         <v>105</v>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Apr-23</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
+      <c r="D29" s="13" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E29" t="n">
         <v>7059</v>
-      </c>
-      <c r="E29" t="n">
-        <v>982.1242499999998</v>
       </c>
       <c r="F29" t="n">
         <v>982.1242499999998</v>
       </c>
       <c r="G29" t="n">
+        <v>982.1242499999998</v>
+      </c>
+      <c r="H29" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30">
+        <f>+C30&amp;"-"&amp;D30</f>
+        <v/>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="C30" t="n">
         <v>105</v>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
+      <c r="D30" s="13" t="n">
+        <v>45047</v>
+      </c>
+      <c r="E30" t="n">
         <v>7235</v>
-      </c>
-      <c r="E30" t="n">
-        <v>1006.67735625</v>
       </c>
       <c r="F30" t="n">
         <v>1006.67735625</v>
       </c>
       <c r="G30" t="n">
+        <v>1006.67735625</v>
+      </c>
+      <c r="H30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31">
+        <f>+C31&amp;"-"&amp;D31</f>
+        <v/>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="C31" t="n">
         <v>105</v>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Jun-23</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
+      <c r="D31" s="13" t="n">
+        <v>45078</v>
+      </c>
+      <c r="E31" t="n">
         <v>7416</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1031.84429015625</v>
       </c>
       <c r="F31" t="n">
         <v>1031.84429015625</v>
       </c>
       <c r="G31" t="n">
+        <v>1031.84429015625</v>
+      </c>
+      <c r="H31" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32">
+        <f>+C32&amp;"-"&amp;D32</f>
+        <v/>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="C32" t="n">
         <v>105</v>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Jul-23</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
+      <c r="D32" s="13" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E32" t="n">
         <v>7602</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1057.640397410156</v>
       </c>
       <c r="F32" t="n">
         <v>1057.640397410156</v>
       </c>
       <c r="G32" t="n">
+        <v>1057.640397410156</v>
+      </c>
+      <c r="H32" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33">
+        <f>+C33&amp;"-"&amp;D33</f>
+        <v/>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="C33" t="n">
         <v>105</v>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Aug-23</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
+      <c r="D33" s="13" t="n">
+        <v>45139</v>
+      </c>
+      <c r="E33" t="n">
         <v>7792</v>
-      </c>
-      <c r="E33" t="n">
-        <v>1084.08140734541</v>
       </c>
       <c r="F33" t="n">
         <v>1084.08140734541</v>
       </c>
       <c r="G33" t="n">
+        <v>1084.08140734541</v>
+      </c>
+      <c r="H33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34">
+        <f>+C34&amp;"-"&amp;D34</f>
+        <v/>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="C34" t="n">
         <v>105</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Sep-23</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
+      <c r="D34" s="13" t="n">
+        <v>45170</v>
+      </c>
+      <c r="E34" t="n">
         <v>7987</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1111.183442529045</v>
       </c>
       <c r="F34" t="n">
         <v>1111.183442529045</v>
       </c>
       <c r="G34" t="n">
+        <v>1111.183442529045</v>
+      </c>
+      <c r="H34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35">
+        <f>+C35&amp;"-"&amp;D35</f>
+        <v/>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="C35" t="n">
         <v>105</v>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Oct-23</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
+      <c r="D35" s="13" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E35" t="n">
         <v>8186</v>
-      </c>
-      <c r="E35" t="n">
-        <v>1138.963028592271</v>
       </c>
       <c r="F35" t="n">
         <v>1138.963028592271</v>
       </c>
       <c r="G35" t="n">
+        <v>1138.963028592271</v>
+      </c>
+      <c r="H35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36">
+        <f>+C36&amp;"-"&amp;D36</f>
+        <v/>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="C36" t="n">
         <v>105</v>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Nov-23</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
+      <c r="D36" s="13" t="n">
+        <v>45231</v>
+      </c>
+      <c r="E36" t="n">
         <v>8391</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1167.437104307078</v>
       </c>
       <c r="F36" t="n">
         <v>1167.437104307078</v>
       </c>
       <c r="G36" t="n">
+        <v>1167.437104307078</v>
+      </c>
+      <c r="H36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37">
+        <f>+C37&amp;"-"&amp;D37</f>
+        <v/>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Annie 7-H</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="C37" t="n">
         <v>105</v>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Dec-23</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
+      <c r="D37" s="13" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E37" t="n">
         <v>8601</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1196.623031914755</v>
       </c>
       <c r="F37" t="n">
         <v>1196.623031914755</v>
       </c>
       <c r="G37" t="n">
+        <v>1196.623031914755</v>
+      </c>
+      <c r="H37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38">
+        <f>+C38&amp;"-"&amp;D38</f>
+        <v/>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="C38" t="n">
         <v>106</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Jan-23</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
+      <c r="D38" s="13" t="n">
+        <v>44927</v>
       </c>
       <c r="E38" t="n">
-        <v>612</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
         <v>612</v>
       </c>
       <c r="G38" t="n">
+        <v>612</v>
+      </c>
+      <c r="H38" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39">
+        <f>+C39&amp;"-"&amp;D39</f>
+        <v/>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="C39" t="n">
         <v>106</v>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Feb-23</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
+      <c r="D39" s="13" t="n">
+        <v>44958</v>
       </c>
       <c r="E39" t="n">
-        <v>627.3</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
         <v>627.3</v>
       </c>
       <c r="G39" t="n">
+        <v>627.3</v>
+      </c>
+      <c r="H39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40">
+        <f>+C40&amp;"-"&amp;D40</f>
+        <v/>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="C40" t="n">
         <v>106</v>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Mar-23</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
+      <c r="D40" s="13" t="n">
+        <v>44986</v>
       </c>
       <c r="E40" t="n">
-        <v>642.9825</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
         <v>642.9825</v>
       </c>
       <c r="G40" t="n">
+        <v>642.9825</v>
+      </c>
+      <c r="H40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41">
+        <f>+C41&amp;"-"&amp;D41</f>
+        <v/>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="C41" t="n">
         <v>106</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Apr-23</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
+      <c r="D41" s="13" t="n">
+        <v>45017</v>
       </c>
       <c r="E41" t="n">
-        <v>659.0570625</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
         <v>659.0570625</v>
       </c>
       <c r="G41" t="n">
+        <v>659.0570625</v>
+      </c>
+      <c r="H41" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42">
+        <f>+C42&amp;"-"&amp;D42</f>
+        <v/>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="C42" t="n">
         <v>106</v>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
+      <c r="D42" s="13" t="n">
+        <v>45047</v>
       </c>
       <c r="E42" t="n">
-        <v>675.5334890624999</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
         <v>675.5334890624999</v>
       </c>
       <c r="G42" t="n">
+        <v>675.5334890624999</v>
+      </c>
+      <c r="H42" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43">
+        <f>+C43&amp;"-"&amp;D43</f>
+        <v/>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="C43" t="n">
         <v>106</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Jun-23</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
+      <c r="D43" s="13" t="n">
+        <v>45078</v>
       </c>
       <c r="E43" t="n">
-        <v>692.4218262890624</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
         <v>692.4218262890624</v>
       </c>
       <c r="G43" t="n">
+        <v>692.4218262890624</v>
+      </c>
+      <c r="H43" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44">
+        <f>+C44&amp;"-"&amp;D44</f>
+        <v/>
+      </c>
+      <c r="B44" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="C44" t="n">
         <v>106</v>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Jul-23</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
+      <c r="D44" s="13" t="n">
+        <v>45108</v>
       </c>
       <c r="E44" t="n">
-        <v>709.7323719462888</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>709.7323719462888</v>
       </c>
       <c r="G44" t="n">
+        <v>709.7323719462888</v>
+      </c>
+      <c r="H44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45">
+        <f>+C45&amp;"-"&amp;D45</f>
+        <v/>
+      </c>
+      <c r="B45" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B45" t="n">
+      <c r="C45" t="n">
         <v>106</v>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Aug-23</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
+      <c r="D45" s="13" t="n">
+        <v>45139</v>
       </c>
       <c r="E45" t="n">
-        <v>727.475681244946</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>727.475681244946</v>
       </c>
       <c r="G45" t="n">
+        <v>727.475681244946</v>
+      </c>
+      <c r="H45" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46">
+        <f>+C46&amp;"-"&amp;D46</f>
+        <v/>
+      </c>
+      <c r="B46" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="C46" t="n">
         <v>106</v>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Sep-23</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
+      <c r="D46" s="13" t="n">
+        <v>45170</v>
       </c>
       <c r="E46" t="n">
-        <v>745.6625732760697</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
         <v>745.6625732760697</v>
       </c>
       <c r="G46" t="n">
+        <v>745.6625732760697</v>
+      </c>
+      <c r="H46" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47">
+        <f>+C47&amp;"-"&amp;D47</f>
+        <v/>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B47" t="n">
+      <c r="C47" t="n">
         <v>106</v>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Oct-23</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
+      <c r="D47" s="13" t="n">
+        <v>45200</v>
       </c>
       <c r="E47" t="n">
-        <v>764.3041376079714</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>764.3041376079714</v>
       </c>
       <c r="G47" t="n">
+        <v>764.3041376079714</v>
+      </c>
+      <c r="H47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48">
+        <f>+C48&amp;"-"&amp;D48</f>
+        <v/>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B48" t="n">
+      <c r="C48" t="n">
         <v>106</v>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Nov-23</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
+      <c r="D48" s="13" t="n">
+        <v>45231</v>
       </c>
       <c r="E48" t="n">
-        <v>783.4117410481706</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
         <v>783.4117410481706</v>
       </c>
       <c r="G48" t="n">
+        <v>783.4117410481706</v>
+      </c>
+      <c r="H48" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49">
+        <f>+C49&amp;"-"&amp;D49</f>
+        <v/>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>Kyle 2-H</t>
         </is>
       </c>
-      <c r="B49" t="n">
+      <c r="C49" t="n">
         <v>106</v>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Dec-23</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
+      <c r="D49" s="13" t="n">
+        <v>45261</v>
       </c>
       <c r="E49" t="n">
-        <v>802.9970345743748</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
         <v>802.9970345743748</v>
       </c>
       <c r="G49" t="n">
+        <v>802.9970345743748</v>
+      </c>
+      <c r="H49" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50">
+        <f>+C50&amp;"-"&amp;D50</f>
+        <v/>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B50" t="n">
+      <c r="C50" t="n">
         <v>107</v>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Jan-23</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
+      <c r="D50" s="13" t="n">
+        <v>44927</v>
+      </c>
+      <c r="E50" t="n">
         <v>7595</v>
-      </c>
-      <c r="E50" t="n">
-        <v>996</v>
       </c>
       <c r="F50" t="n">
         <v>996</v>
       </c>
       <c r="G50" t="n">
+        <v>996</v>
+      </c>
+      <c r="H50" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51">
+        <f>+C51&amp;"-"&amp;D51</f>
+        <v/>
+      </c>
+      <c r="B51" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B51" t="n">
+      <c r="C51" t="n">
         <v>107</v>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Feb-23</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
+      <c r="D51" s="13" t="n">
+        <v>44958</v>
+      </c>
+      <c r="E51" t="n">
         <v>7784</v>
-      </c>
-      <c r="E51" t="n">
-        <v>1020.9</v>
       </c>
       <c r="F51" t="n">
         <v>1020.9</v>
       </c>
       <c r="G51" t="n">
+        <v>1020.9</v>
+      </c>
+      <c r="H51" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52">
+        <f>+C52&amp;"-"&amp;D52</f>
+        <v/>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B52" t="n">
+      <c r="C52" t="n">
         <v>107</v>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Mar-23</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
+      <c r="D52" s="13" t="n">
+        <v>44986</v>
+      </c>
+      <c r="E52" t="n">
         <v>7979</v>
-      </c>
-      <c r="E52" t="n">
-        <v>1046.4225</v>
       </c>
       <c r="F52" t="n">
         <v>1046.4225</v>
       </c>
       <c r="G52" t="n">
+        <v>1046.4225</v>
+      </c>
+      <c r="H52" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53">
+        <f>+C53&amp;"-"&amp;D53</f>
+        <v/>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="C53" t="n">
         <v>107</v>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Apr-23</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
+      <c r="D53" s="13" t="n">
+        <v>45017</v>
+      </c>
+      <c r="E53" t="n">
         <v>8178</v>
-      </c>
-      <c r="E53" t="n">
-        <v>1072.5830625</v>
       </c>
       <c r="F53" t="n">
         <v>1072.5830625</v>
       </c>
       <c r="G53" t="n">
+        <v>1072.5830625</v>
+      </c>
+      <c r="H53" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54">
+        <f>+C54&amp;"-"&amp;D54</f>
+        <v/>
+      </c>
+      <c r="B54" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B54" t="n">
+      <c r="C54" t="n">
         <v>107</v>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
+      <c r="D54" s="13" t="n">
+        <v>45047</v>
+      </c>
+      <c r="E54" t="n">
         <v>8383</v>
-      </c>
-      <c r="E54" t="n">
-        <v>1099.3976390625</v>
       </c>
       <c r="F54" t="n">
         <v>1099.3976390625</v>
       </c>
       <c r="G54" t="n">
+        <v>1099.3976390625</v>
+      </c>
+      <c r="H54" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55">
+        <f>+C55&amp;"-"&amp;D55</f>
+        <v/>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B55" t="n">
+      <c r="C55" t="n">
         <v>107</v>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Jun-23</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
+      <c r="D55" s="13" t="n">
+        <v>45078</v>
+      </c>
+      <c r="E55" t="n">
         <v>8592</v>
-      </c>
-      <c r="E55" t="n">
-        <v>1126.882580039062</v>
       </c>
       <c r="F55" t="n">
         <v>1126.882580039062</v>
       </c>
       <c r="G55" t="n">
+        <v>1126.882580039062</v>
+      </c>
+      <c r="H55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56">
+        <f>+C56&amp;"-"&amp;D56</f>
+        <v/>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B56" t="n">
+      <c r="C56" t="n">
         <v>107</v>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Jul-23</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
+      <c r="D56" s="13" t="n">
+        <v>45108</v>
+      </c>
+      <c r="E56" t="n">
         <v>8807</v>
-      </c>
-      <c r="E56" t="n">
-        <v>1155.054644540039</v>
       </c>
       <c r="F56" t="n">
         <v>1155.054644540039</v>
       </c>
       <c r="G56" t="n">
+        <v>1155.054644540039</v>
+      </c>
+      <c r="H56" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57">
+        <f>+C57&amp;"-"&amp;D57</f>
+        <v/>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B57" t="n">
+      <c r="C57" t="n">
         <v>107</v>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Aug-23</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
+      <c r="D57" s="13" t="n">
+        <v>45139</v>
+      </c>
+      <c r="E57" t="n">
         <v>9027</v>
-      </c>
-      <c r="E57" t="n">
-        <v>1183.93101065354</v>
       </c>
       <c r="F57" t="n">
         <v>1183.93101065354</v>
       </c>
       <c r="G57" t="n">
+        <v>1183.93101065354</v>
+      </c>
+      <c r="H57" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58">
+        <f>+C58&amp;"-"&amp;D58</f>
+        <v/>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B58" t="n">
+      <c r="C58" t="n">
         <v>107</v>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Sep-23</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
+      <c r="D58" s="13" t="n">
+        <v>45170</v>
+      </c>
+      <c r="E58" t="n">
         <v>9253</v>
-      </c>
-      <c r="E58" t="n">
-        <v>1213.529285919878</v>
       </c>
       <c r="F58" t="n">
         <v>1213.529285919878</v>
       </c>
       <c r="G58" t="n">
+        <v>1213.529285919878</v>
+      </c>
+      <c r="H58" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59">
+        <f>+C59&amp;"-"&amp;D59</f>
+        <v/>
+      </c>
+      <c r="B59" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B59" t="n">
+      <c r="C59" t="n">
         <v>107</v>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Oct-23</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
+      <c r="D59" s="13" t="n">
+        <v>45200</v>
+      </c>
+      <c r="E59" t="n">
         <v>9484</v>
-      </c>
-      <c r="E59" t="n">
-        <v>1243.867518067875</v>
       </c>
       <c r="F59" t="n">
         <v>1243.867518067875</v>
       </c>
       <c r="G59" t="n">
+        <v>1243.867518067875</v>
+      </c>
+      <c r="H59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60">
+        <f>+C60&amp;"-"&amp;D60</f>
+        <v/>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B60" t="n">
+      <c r="C60" t="n">
         <v>107</v>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Nov-23</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
+      <c r="D60" s="13" t="n">
+        <v>45231</v>
+      </c>
+      <c r="E60" t="n">
         <v>9722</v>
-      </c>
-      <c r="E60" t="n">
-        <v>1274.964206019572</v>
       </c>
       <c r="F60" t="n">
         <v>1274.964206019572</v>
       </c>
       <c r="G60" t="n">
+        <v>1274.964206019572</v>
+      </c>
+      <c r="H60" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61">
+        <f>+C61&amp;"-"&amp;D61</f>
+        <v/>
+      </c>
+      <c r="B61" t="inlineStr">
         <is>
           <t>Eric 2-H</t>
         </is>
       </c>
-      <c r="B61" t="n">
+      <c r="C61" t="n">
         <v>107</v>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Dec-23</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
+      <c r="D61" s="13" t="n">
+        <v>45261</v>
+      </c>
+      <c r="E61" t="n">
         <v>9965</v>
-      </c>
-      <c r="E61" t="n">
-        <v>1306.838311170061</v>
       </c>
       <c r="F61" t="n">
         <v>1306.838311170061</v>
       </c>
       <c r="G61" t="n">
+        <v>1306.838311170061</v>
+      </c>
+      <c r="H61" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>